<commit_message>
Prob modèle pas si pire mais problème de nan
</commit_message>
<xml_diff>
--- a/APP3/code_problematique_2024/Itérations_prob.xlsx
+++ b/APP3/code_problematique_2024/Itérations_prob.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\Documents\UNIVERSITÉ\COURS\S7\github\S7\APP3\code_problematique_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01FEBB4-10BB-451E-A50B-5A0F3CDAD2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8436A336-6473-4F57-BF12-E787A9E50734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4815" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4815" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>Variations</t>
   </si>
@@ -107,12 +108,18 @@
   <si>
     <t>GRU + attn</t>
   </si>
+  <si>
+    <t>nan 91</t>
+  </si>
+  <si>
+    <t>nan 100</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +152,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -271,36 +284,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
@@ -1206,6 +1217,539 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>3063647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8FFFA77-85FC-CEE7-5DD1-A6660287E44D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3038476" y="4572000"/>
+          <a:ext cx="4095750" cy="3063647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>483982</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>3089219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EA501F6-9381-145B-6F2A-661C6EE767EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7439024" y="4648200"/>
+          <a:ext cx="2179433" cy="3013019"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>346553</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>3133725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC76DA1F-276F-9196-E6F9-1ADDE06653B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3057526" y="7696201"/>
+          <a:ext cx="4137502" cy="3114674"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>3170813</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6C410A1-BD69-02C8-86E7-914C59DBBC94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7400926" y="7696201"/>
+          <a:ext cx="2286000" cy="3151762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>321900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>3095625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEA48F7E-D0C4-8432-7703-8737363B42CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3038475" y="13954125"/>
+          <a:ext cx="4131900" cy="3095625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>452009</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>629325</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>3238500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{135ACCA0-A40F-97D2-DD44-F8D744187335}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7300484" y="14011650"/>
+          <a:ext cx="2463316" cy="3180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>3314700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>2871864</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4182C0D6-7C05-0D3F-880C-1BD14DBAE84A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3162300" y="17268825"/>
+          <a:ext cx="3733800" cy="2881389"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>372094</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>48296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{612FB44C-80B0-0199-29AB-1ADC8CDCFBBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7324724" y="17306925"/>
+          <a:ext cx="2181845" cy="3010571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1376261</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>508655</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>3362325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0200C8F7-057D-995F-3FA3-1743982CE9B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2900261" y="20269200"/>
+          <a:ext cx="4456869" cy="3362325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514078</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>599328</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>3343275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Image 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD736C40-A318-B96A-5FF4-84C8F189AAF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7362553" y="20402551"/>
+          <a:ext cx="2371250" cy="3209924"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>3496586</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E3D7C97-264E-D346-BB89-A79F6D524E77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2847975" y="23650576"/>
+          <a:ext cx="4600575" cy="3487060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>3352801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>353066</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>3525227</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Image 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{459A9E53-4F58-D807-BE56-D78ED95EECDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7600950" y="23622001"/>
+          <a:ext cx="2648591" cy="3544276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1471,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,30 +2026,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
@@ -1546,8 +2090,8 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D5">
@@ -1588,8 +2132,8 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D6">
@@ -1630,8 +2174,8 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D7">
@@ -1672,8 +2216,8 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D8">
@@ -1714,10 +2258,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="2">
@@ -1759,137 +2303,134 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P10" s="3"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11">
         <v>64</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11">
         <v>64</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11">
         <v>64</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11">
         <v>64</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11">
         <v>64</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11">
         <v>64</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11">
         <v>64</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11">
         <v>64</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11">
         <v>64</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11">
         <v>64</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11">
         <v>64</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11">
         <v>64</v>
       </c>
-      <c r="P11" s="3"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12">
         <v>15</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12">
         <v>15</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12">
         <v>15</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12">
         <v>15</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12">
         <v>15</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12">
         <v>15</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12">
         <v>15</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12">
         <v>15</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12">
         <v>15</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12">
         <v>15</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12">
         <v>15</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12">
         <v>9</v>
       </c>
-      <c r="P12" s="3"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="1">
@@ -1931,156 +2472,156 @@
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="7">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
-      <c r="H14" s="7">
-        <v>1</v>
-      </c>
-      <c r="I14" s="7">
-        <v>1</v>
-      </c>
-      <c r="J14" s="7">
-        <v>1</v>
-      </c>
-      <c r="K14" s="7">
-        <v>0</v>
-      </c>
-      <c r="L14" s="7">
-        <v>0</v>
-      </c>
-      <c r="M14" s="7">
-        <v>0</v>
-      </c>
-      <c r="N14" s="7">
-        <v>0</v>
-      </c>
-      <c r="O14" s="7">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7">
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
-        <v>1</v>
-      </c>
-      <c r="L15" s="7">
-        <v>1</v>
-      </c>
-      <c r="M15" s="7">
-        <v>0</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0</v>
-      </c>
-      <c r="O15" s="7">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7">
-        <v>0</v>
-      </c>
-      <c r="J16" s="7">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7">
-        <v>0</v>
-      </c>
-      <c r="L16" s="7">
-        <v>0</v>
-      </c>
-      <c r="M16" s="7">
-        <v>1</v>
-      </c>
-      <c r="N16" s="7">
-        <v>1</v>
-      </c>
-      <c r="O16" s="7">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D19">
@@ -2121,10 +2662,10 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="10">
         <v>8504</v>
       </c>
       <c r="E20">
@@ -2133,36 +2674,36 @@
       <c r="F20">
         <v>31319</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="12">
         <v>16094</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="11">
         <v>45554</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="10">
         <v>9209</v>
       </c>
       <c r="J20">
         <v>24419</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="10">
         <v>8504</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="10">
         <v>9209</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="10">
         <v>8504</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N20" s="10">
         <v>9209</v>
       </c>
-      <c r="O20" s="18">
+      <c r="O20" s="10">
         <v>9605</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D21">
@@ -2197,7 +2738,7 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D22">
@@ -2237,90 +2778,90 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="17">
+      <c r="B27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="251.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="244.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="240" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="264" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="17">
+      <c r="B34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9">
         <v>8</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="276" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="17">
+      <c r="B36" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="237" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="9">
         <v>11</v>
       </c>
     </row>
@@ -2335,4 +2876,595 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200FBD0-4DB8-4AB7-9EB6-C4D4F32A5EB3}">
+  <dimension ref="B2:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="13"/>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>100</v>
+      </c>
+      <c r="F8" s="2">
+        <v>100</v>
+      </c>
+      <c r="G8" s="2">
+        <v>100</v>
+      </c>
+      <c r="H8" s="2">
+        <v>100</v>
+      </c>
+      <c r="I8" s="2">
+        <v>200</v>
+      </c>
+      <c r="J8" s="2">
+        <v>200</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.03</v>
+      </c>
+      <c r="G9">
+        <v>0.03</v>
+      </c>
+      <c r="H9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="J9">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="13"/>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <v>80</v>
+      </c>
+      <c r="G10">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>80</v>
+      </c>
+      <c r="I10">
+        <v>80</v>
+      </c>
+      <c r="J10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>18</v>
+      </c>
+      <c r="H11">
+        <v>18</v>
+      </c>
+      <c r="I11">
+        <v>18</v>
+      </c>
+      <c r="J11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="19">
+        <v>9425</v>
+      </c>
+      <c r="E19" s="20">
+        <v>9659</v>
+      </c>
+      <c r="F19" s="20">
+        <v>9659</v>
+      </c>
+      <c r="G19" s="19">
+        <v>9425</v>
+      </c>
+      <c r="H19" s="19">
+        <v>9425</v>
+      </c>
+      <c r="I19" s="19">
+        <v>9425</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="E20">
+        <v>1.85</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20">
+        <v>1.831</v>
+      </c>
+      <c r="I20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>2.3530000000000002</v>
+      </c>
+      <c r="E21">
+        <v>2.915</v>
+      </c>
+      <c r="G21">
+        <v>2.9350000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="244.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="237" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="261.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="235.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="265.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="285.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="9">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D2:P2"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>